<commit_message>
add res boundary attack for SEED 7
</commit_message>
<xml_diff>
--- a/results/SEED_7/result.xlsx
+++ b/results/SEED_7/result.xlsx
@@ -474,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR12"/>
+  <dimension ref="A1:AZ12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -558,6 +558,18 @@
       <c r="AP1" s="1" t="n"/>
       <c r="AQ1" s="1" t="n"/>
       <c r="AR1" s="1" t="n"/>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>BOUNDARY</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="n"/>
+      <c r="AU1" s="1" t="n"/>
+      <c r="AV1" s="1" t="n"/>
+      <c r="AW1" s="1" t="n"/>
+      <c r="AX1" s="1" t="n"/>
+      <c r="AY1" s="1" t="n"/>
+      <c r="AZ1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="B2" s="1" t="inlineStr">
@@ -775,6 +787,46 @@
           <t>0.20</t>
         </is>
       </c>
+      <c r="AS2" s="1" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="AT2" s="1" t="inlineStr">
+        <is>
+          <t>0.02</t>
+        </is>
+      </c>
+      <c r="AU2" s="1" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="AV2" s="1" t="inlineStr">
+        <is>
+          <t>0.04</t>
+        </is>
+      </c>
+      <c r="AW2" s="1" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="AX2" s="1" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+      <c r="AY2" s="1" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+      <c r="AZ2" s="1" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -924,6 +976,30 @@
       </c>
       <c r="AR4" t="n">
         <v>31.74152755737305</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>5.686472415924072</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>5.738160610198975</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>5.786428451538086</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>5.824905395507812</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>5.838682174682617</v>
+      </c>
+      <c r="AX4" t="n">
+        <v>6.180508613586426</v>
+      </c>
+      <c r="AY4" t="n">
+        <v>6.379770278930664</v>
+      </c>
+      <c r="AZ4" t="n">
+        <v>8.032449722290039</v>
       </c>
     </row>
     <row r="5">
@@ -1059,6 +1135,30 @@
       <c r="AR5" t="n">
         <v>32.0003795601269</v>
       </c>
+      <c r="AS5" t="n">
+        <v>6.940323538590438</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>6.971137078464893</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>7.02943390174514</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>7.062481095280284</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>7.058417836854031</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>7.450958640870901</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>7.716292634911398</v>
+      </c>
+      <c r="AZ5" t="n">
+        <v>10.01064954176535</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
@@ -1193,6 +1293,30 @@
       <c r="AR6" t="n">
         <v>0.9895968437194824</v>
       </c>
+      <c r="AS6" t="n">
+        <v>0.9995881319046021</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>0.99958735704422</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>0.9995734691619873</v>
+      </c>
+      <c r="AV6" t="n">
+        <v>0.9995725154876709</v>
+      </c>
+      <c r="AW6" t="n">
+        <v>0.9995645880699158</v>
+      </c>
+      <c r="AX6" t="n">
+        <v>0.9995023012161255</v>
+      </c>
+      <c r="AY6" t="n">
+        <v>0.9994622468948364</v>
+      </c>
+      <c r="AZ6" t="n">
+        <v>0.9989767074584961</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1330,6 +1454,30 @@
       </c>
       <c r="AR7" t="n">
         <v>42.70527267456055</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>5.008236408233643</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>5.140683650970459</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>5.160590648651123</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>5.451739311218262</v>
+      </c>
+      <c r="AW7" t="n">
+        <v>5.69630241394043</v>
+      </c>
+      <c r="AX7" t="n">
+        <v>6.743438720703125</v>
+      </c>
+      <c r="AY7" t="n">
+        <v>8.162350654602051</v>
+      </c>
+      <c r="AZ7" t="n">
+        <v>12.6733283996582</v>
       </c>
     </row>
     <row r="8">
@@ -1465,6 +1613,30 @@
       <c r="AR8" t="n">
         <v>42.83441643638107</v>
       </c>
+      <c r="AS8" t="n">
+        <v>5.947171656174707</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>6.109762740453094</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>6.155543872594171</v>
+      </c>
+      <c r="AV8" t="n">
+        <v>6.425935301629828</v>
+      </c>
+      <c r="AW8" t="n">
+        <v>6.895325180031679</v>
+      </c>
+      <c r="AX8" t="n">
+        <v>8.271070910932385</v>
+      </c>
+      <c r="AY8" t="n">
+        <v>10.15984799549205</v>
+      </c>
+      <c r="AZ8" t="n">
+        <v>15.88342398063569</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
@@ -1599,6 +1771,30 @@
       <c r="AR9" t="n">
         <v>0.987388551235199</v>
       </c>
+      <c r="AS9" t="n">
+        <v>0.9997783303260803</v>
+      </c>
+      <c r="AT9" t="n">
+        <v>0.9997398257255554</v>
+      </c>
+      <c r="AU9" t="n">
+        <v>0.9997555017471313</v>
+      </c>
+      <c r="AV9" t="n">
+        <v>0.9996582865715027</v>
+      </c>
+      <c r="AW9" t="n">
+        <v>0.9995759129524231</v>
+      </c>
+      <c r="AX9" t="n">
+        <v>0.9991956353187561</v>
+      </c>
+      <c r="AY9" t="n">
+        <v>0.9986026287078857</v>
+      </c>
+      <c r="AZ9" t="n">
+        <v>0.9958498477935791</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1736,6 +1932,30 @@
       </c>
       <c r="AR10" t="n">
         <v>30.5800895690918</v>
+      </c>
+      <c r="AS10" t="n">
+        <v>2.663012027740479</v>
+      </c>
+      <c r="AT10" t="n">
+        <v>2.788084268569946</v>
+      </c>
+      <c r="AU10" t="n">
+        <v>3.055869340896606</v>
+      </c>
+      <c r="AV10" t="n">
+        <v>3.33517599105835</v>
+      </c>
+      <c r="AW10" t="n">
+        <v>3.796853542327881</v>
+      </c>
+      <c r="AX10" t="n">
+        <v>4.766287803649902</v>
+      </c>
+      <c r="AY10" t="n">
+        <v>5.873990058898926</v>
+      </c>
+      <c r="AZ10" t="n">
+        <v>9.78786563873291</v>
       </c>
     </row>
     <row r="11">
@@ -1871,6 +2091,30 @@
       <c r="AR11" t="n">
         <v>30.79464829754565</v>
       </c>
+      <c r="AS11" t="n">
+        <v>3.583970138978879</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>3.709712354300256</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>3.937894407833777</v>
+      </c>
+      <c r="AV11" t="n">
+        <v>4.300472792426818</v>
+      </c>
+      <c r="AW11" t="n">
+        <v>4.849296298543166</v>
+      </c>
+      <c r="AX11" t="n">
+        <v>6.057199579677631</v>
+      </c>
+      <c r="AY11" t="n">
+        <v>7.353330425954725</v>
+      </c>
+      <c r="AZ11" t="n">
+        <v>12.35969969350679</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
@@ -2005,9 +2249,33 @@
       <c r="AR12" t="n">
         <v>0.9830489158630371</v>
       </c>
+      <c r="AS12" t="n">
+        <v>0.9997842311859131</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>0.999767005443573</v>
+      </c>
+      <c r="AU12" t="n">
+        <v>0.9997367262840271</v>
+      </c>
+      <c r="AV12" t="n">
+        <v>0.9996891021728516</v>
+      </c>
+      <c r="AW12" t="n">
+        <v>0.9995875954627991</v>
+      </c>
+      <c r="AX12" t="n">
+        <v>0.9993520379066467</v>
+      </c>
+      <c r="AY12" t="n">
+        <v>0.9990388154983521</v>
+      </c>
+      <c r="AZ12" t="n">
+        <v>0.9973019957542419</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="M1:T1"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A9"/>
@@ -2016,6 +2284,7 @@
     <mergeCell ref="AC1:AJ1"/>
     <mergeCell ref="AK1:AR1"/>
     <mergeCell ref="U1:AB1"/>
+    <mergeCell ref="AS1:AZ1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>